<commit_message>
v0.2, input from first demo, other improvements
</commit_message>
<xml_diff>
--- a/inputs/template.xlsx
+++ b/inputs/template.xlsx
@@ -16,9 +16,10 @@
     <sheet name="Units" sheetId="6" state="visible" r:id="rId7"/>
     <sheet name="Uncertainty" sheetId="7" state="visible" r:id="rId8"/>
     <sheet name="Defaults" sheetId="8" state="visible" r:id="rId9"/>
-    <sheet name="Directories" sheetId="9" state="visible" r:id="rId10"/>
-    <sheet name="Names" sheetId="10" state="hidden" r:id="rId11"/>
-    <sheet name="Options" sheetId="11" state="hidden" r:id="rId12"/>
+    <sheet name="Reproducibility" sheetId="9" state="visible" r:id="rId10"/>
+    <sheet name="Directories" sheetId="10" state="visible" r:id="rId11"/>
+    <sheet name="Names" sheetId="11" state="hidden" r:id="rId12"/>
+    <sheet name="Options" sheetId="12" state="hidden" r:id="rId13"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -32,22 +33,9 @@
 <file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
-    <author>SH</author>
+    <author>SDH</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">Arbitrary name for application event that user can recognize</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="B1" authorId="0">
       <text>
         <r>
@@ -66,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="178">
   <si>
     <t xml:space="preserve">Combined input file for the ALFAMI R package for estimation of ammonia emission from field-applied slurry</t>
   </si>
@@ -120,6 +108,12 @@
   </si>
   <si>
     <t xml:space="preserve">Optional: enter or check default inputs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reproducibility</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Avoid if possible: change settings related to reproducibility if necessary</t>
   </si>
   <si>
     <t xml:space="preserve">Directories</t>
@@ -163,6 +157,9 @@
     <t xml:space="preserve">Keys must match between sheets</t>
   </si>
   <si>
+    <t xml:space="preserve">Setting accessible only for reproducibility—users should change only if necessary</t>
+  </si>
+  <si>
     <t xml:space="preserve">Unit set in “Units" sheet</t>
   </si>
   <si>
@@ -202,7 +199,7 @@
     <t xml:space="preserve">pH</t>
   </si>
   <si>
-    <t xml:space="preserve">Application name</t>
+    <t xml:space="preserve">Application event name</t>
   </si>
   <si>
     <t xml:space="preserve">Application year</t>
@@ -256,157 +253,169 @@
     <t xml:space="preserve">Value</t>
   </si>
   <si>
+    <t xml:space="preserve">Include input uncertainty?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Include par uncertainty?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uncertainty iterations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Confidence level</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Weather resolution</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Monthly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Output digits</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Output file name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Overwrite output?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Type of output</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xlsx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Variable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Notes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Slurry mass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">t</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TAN mass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Land area</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ha</t>
+  </si>
+  <si>
+    <t xml:space="preserve">t/ha</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Slurry dry matter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">% FM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">% of fresh mass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TAN concentration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kg/t</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Air temperature</t>
+  </si>
+  <si>
+    <t xml:space="preserve">°C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wind speed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m/s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">`</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Input</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Absolute uncertainty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Relative uncertainty (frac.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lower limit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Upper limit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Slurry pH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Default value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Source</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Application day of month</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Assumed, middle of month</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Application time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HH:MM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">09:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Assumed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Average from ALFAM2 database vx.x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Slurry TAN</t>
+  </si>
+  <si>
     <t xml:space="preserve">Parameter set</t>
   </si>
   <si>
     <t xml:space="preserve">ALFAM2pars02</t>
   </si>
   <si>
-    <t xml:space="preserve">Include input uncertainty?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Include par uncertainty?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Uncertainty iterations</t>
-  </si>
-  <si>
     <t xml:space="preserve">Uncertainty seed</t>
   </si>
   <si>
-    <t xml:space="preserve">Confidence level</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Weather type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Constant</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Output digits</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Output file name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Overwrite output?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Type of output</t>
-  </si>
-  <si>
-    <t xml:space="preserve">xlsx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Variable</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Notes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Slurry mass</t>
-  </si>
-  <si>
-    <t xml:space="preserve">t</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TAN mass</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Land area</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ha</t>
-  </si>
-  <si>
-    <t xml:space="preserve">t/ha</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Slurry dry matter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">% FM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">% of fresh mass</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TAN concentration</t>
-  </si>
-  <si>
-    <t xml:space="preserve">kg/t</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Time</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Air temperature</t>
-  </si>
-  <si>
-    <t xml:space="preserve">°C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wind speed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">m/s</t>
-  </si>
-  <si>
-    <t xml:space="preserve">`</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Input</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Absolute uncertainty</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Relative uncertainty (frac.)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lower limit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Upper limit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Slurry pH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Default value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Application day of month</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Application time</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HH:MM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">09:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Emission duration</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Slurry TAN</t>
+    <t xml:space="preserve">Emission duration (h)</t>
   </si>
   <si>
     <t xml:space="preserve">File type</t>
@@ -502,42 +511,42 @@
     <t xml:space="preserve">wthr.time</t>
   </si>
   <si>
+    <t xml:space="preserve">uncert</t>
+  </si>
+  <si>
+    <t xml:space="preserve">paruncert</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wthr.type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ndig</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ofile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">overwrite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">otype</t>
+  </si>
+  <si>
+    <t xml:space="preserve">parset</t>
+  </si>
+  <si>
+    <t xml:space="preserve">seedu</t>
+  </si>
+  <si>
     <t xml:space="preserve">emis.dur</t>
   </si>
   <si>
-    <t xml:space="preserve">parset</t>
-  </si>
-  <si>
-    <t xml:space="preserve">uncert</t>
-  </si>
-  <si>
-    <t xml:space="preserve">paruncert</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">seedu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cl</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wthr.type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ndig</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ofile</t>
-  </si>
-  <si>
-    <t xml:space="preserve">overwrite</t>
-  </si>
-  <si>
-    <t xml:space="preserve">otype</t>
-  </si>
-  <si>
     <t xml:space="preserve">Application methods</t>
   </si>
   <si>
@@ -574,6 +583,9 @@
     <t xml:space="preserve">Deep</t>
   </si>
   <si>
+    <t xml:space="preserve">Daily</t>
+  </si>
+  <si>
     <t xml:space="preserve">CSV2</t>
   </si>
   <si>
@@ -581,6 +593,9 @@
   </si>
   <si>
     <t xml:space="preserve">ALFAM2pars03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sub-daily</t>
   </si>
   <si>
     <t xml:space="preserve">Open slot injection</t>
@@ -605,7 +620,7 @@
     <numFmt numFmtId="166" formatCode="General"/>
     <numFmt numFmtId="167" formatCode="hh:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="17">
+  <fonts count="18">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -722,6 +737,13 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF8000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -855,7 +877,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="66">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -980,103 +1002,119 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1159,7 +1197,7 @@
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
       <rgbColor rgb="FFFFCC00"/>
-      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF8000"/>
       <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF666666"/>
       <rgbColor rgb="FF969696"/>
@@ -1181,10 +1219,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B2:D19"/>
+  <dimension ref="B2:D21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
+      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1277,51 +1315,67 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="4" t="s">
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D13" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="4" t="s">
         <v>22</v>
       </c>
+      <c r="D15" s="4" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D16" s="1" t="s">
+      <c r="B16" s="5" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="6" t="s">
         <v>25</v>
       </c>
+      <c r="D17" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="8" t="s">
-        <v>26</v>
+      <c r="B18" s="6" t="s">
+        <v>25</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D19" s="1" t="s">
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="8" t="s">
         <v>29</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B18" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B20" type="list">
       <formula1>"Select input from list"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -1341,15 +1395,75 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O44"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A19" activeCellId="0" sqref="A19"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.65234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.08"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="2" style="1" width="11.64"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="35" t="s">
+        <v>116</v>
+      </c>
+      <c r="B2" s="36" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="37" t="s">
+        <v>118</v>
+      </c>
+      <c r="B3" s="38" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="40" t="s">
+        <v>120</v>
+      </c>
+      <c r="B4" s="41" t="s">
+        <v>121</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:O41"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E21" activeCellId="0" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="56" width="26.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="60" width="26.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="18" width="19.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="18" width="11.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="18" width="16.99"/>
@@ -1366,9 +1480,9 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="16" style="18" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" s="58" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="57" t="s">
-        <v>115</v>
+    <row r="1" s="62" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="61" t="s">
+        <v>122</v>
       </c>
       <c r="B1" s="18"/>
       <c r="C1" s="18"/>
@@ -1379,48 +1493,48 @@
       <c r="H1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="59" t="str">
+      <c r="A2" s="63" t="str">
         <f aca="false">Locations!A1</f>
         <v>Location key</v>
       </c>
-      <c r="B2" s="58" t="str">
+      <c r="B2" s="62" t="str">
         <f aca="false">Locations!B1</f>
         <v>Aggregation group 1</v>
       </c>
-      <c r="C2" s="58" t="str">
+      <c r="C2" s="62" t="str">
         <f aca="false">Locations!C1</f>
         <v>Aggregation group 2</v>
       </c>
-      <c r="D2" s="58" t="str">
+      <c r="D2" s="62" t="str">
         <f aca="false">Locations!D1</f>
         <v>Description</v>
       </c>
-      <c r="E2" s="58"/>
-      <c r="F2" s="58"/>
-      <c r="G2" s="58"/>
-      <c r="H2" s="58"/>
-      <c r="I2" s="58"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
+      <c r="G2" s="62"/>
+      <c r="H2" s="62"/>
+      <c r="I2" s="62"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="56" t="s">
-        <v>116</v>
+      <c r="A3" s="60" t="s">
+        <v>123</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>117</v>
+        <v>124</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>118</v>
+        <v>125</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>119</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="10"/>
       <c r="C4" s="10"/>
     </row>
-    <row r="5" s="58" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="57" t="s">
+    <row r="5" s="62" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="61" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="18"/>
@@ -1430,47 +1544,47 @@
       <c r="F5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="59" t="str">
+      <c r="A6" s="63" t="str">
         <f aca="false">'Slurry composition'!A1</f>
         <v>Slurry key</v>
       </c>
-      <c r="B6" s="58" t="str">
+      <c r="B6" s="62" t="str">
         <f aca="false">'Slurry composition'!B1</f>
         <v>Animal</v>
       </c>
-      <c r="C6" s="58" t="str">
+      <c r="C6" s="62" t="str">
         <f aca="false">'Slurry composition'!C1</f>
         <v>Dry matter</v>
       </c>
-      <c r="D6" s="58" t="str">
+      <c r="D6" s="62" t="str">
         <f aca="false">'Slurry composition'!D1</f>
         <v>TAN</v>
       </c>
-      <c r="E6" s="58" t="str">
+      <c r="E6" s="62" t="str">
         <f aca="false">'Slurry composition'!E1</f>
         <v>pH</v>
       </c>
       <c r="F6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="56" t="s">
-        <v>120</v>
+      <c r="A7" s="60" t="s">
+        <v>127</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>121</v>
+        <v>128</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>122</v>
+        <v>129</v>
       </c>
       <c r="D7" s="18" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="E7" s="18" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="9" s="58" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="57" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="9" s="62" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="61" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="18"/>
@@ -1488,304 +1602,295 @@
       <c r="N9" s="0"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="59" t="str">
+      <c r="A10" s="63" t="str">
         <f aca="false">Application!A1</f>
-        <v>Application name</v>
-      </c>
-      <c r="B10" s="58" t="str">
+        <v>Application event name</v>
+      </c>
+      <c r="B10" s="62" t="str">
         <f aca="false">Application!B1</f>
         <v>Location key</v>
       </c>
-      <c r="C10" s="58" t="str">
+      <c r="C10" s="62" t="str">
         <f aca="false">Application!C1</f>
         <v>Application year</v>
       </c>
-      <c r="D10" s="58" t="str">
+      <c r="D10" s="62" t="str">
         <f aca="false">Application!D1</f>
         <v>Slurry key</v>
       </c>
-      <c r="E10" s="58" t="str">
+      <c r="E10" s="62" t="str">
         <f aca="false">Application!E1</f>
         <v>Slurry application</v>
       </c>
-      <c r="F10" s="58" t="str">
+      <c r="F10" s="62" t="str">
         <f aca="false">Application!F1</f>
         <v>TAN application</v>
       </c>
-      <c r="G10" s="58" t="str">
+      <c r="G10" s="62" t="str">
         <f aca="false">Application!G1</f>
         <v>Application area</v>
       </c>
-      <c r="H10" s="58" t="str">
+      <c r="H10" s="62" t="str">
         <f aca="false">Application!H1</f>
         <v>Application rate</v>
       </c>
-      <c r="I10" s="58" t="str">
+      <c r="I10" s="62" t="str">
         <f aca="false">Application!I1</f>
         <v>Application method</v>
       </c>
-      <c r="J10" s="58" t="str">
+      <c r="J10" s="62" t="str">
         <f aca="false">Application!J1</f>
         <v>Incorporation</v>
       </c>
-      <c r="K10" s="58" t="str">
+      <c r="K10" s="62" t="str">
         <f aca="false">Application!K1</f>
         <v>Incorporation delay</v>
       </c>
-      <c r="L10" s="58" t="str">
+      <c r="L10" s="62" t="str">
         <f aca="false">Application!L1</f>
         <v>Weather year</v>
       </c>
-      <c r="M10" s="58" t="str">
+      <c r="M10" s="62" t="str">
         <f aca="false">Application!M1</f>
         <v>Application month</v>
       </c>
-      <c r="N10" s="58" t="str">
+      <c r="N10" s="62" t="str">
         <f aca="false">Application!N1</f>
         <v>Application day</v>
       </c>
-      <c r="O10" s="58"/>
+      <c r="O10" s="62"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="56" t="s">
-        <v>125</v>
+      <c r="A11" s="60" t="s">
+        <v>132</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>126</v>
+        <v>133</v>
       </c>
       <c r="D11" s="18" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="E11" s="18" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>128</v>
+        <v>135</v>
       </c>
       <c r="G11" s="18" t="s">
-        <v>129</v>
+        <v>136</v>
       </c>
       <c r="H11" s="18" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
       <c r="I11" s="18" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
       <c r="J11" s="18" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
       <c r="K11" s="18" t="s">
-        <v>133</v>
+        <v>140</v>
       </c>
       <c r="L11" s="18" t="s">
-        <v>134</v>
+        <v>141</v>
       </c>
       <c r="M11" s="18" t="s">
-        <v>135</v>
+        <v>142</v>
       </c>
       <c r="N11" s="18" t="s">
-        <v>136</v>
+        <v>143</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F12" s="0"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="57" t="s">
+      <c r="A13" s="61" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="59" t="str">
+      <c r="A14" s="63" t="str">
         <f aca="false">Defaults!A2</f>
         <v>Application day of month</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>136</v>
-      </c>
-      <c r="C14" s="58"/>
-      <c r="D14" s="58"/>
+        <v>143</v>
+      </c>
+      <c r="C14" s="62"/>
+      <c r="D14" s="62"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="60" t="str">
+      <c r="A15" s="64" t="str">
         <f aca="false">Defaults!A3</f>
         <v>Application time</v>
       </c>
       <c r="B15" s="10" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="63" t="str">
+        <f aca="false">Defaults!A4</f>
+        <v>Application rate</v>
+      </c>
+      <c r="B16" s="18" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="59" t="str">
-        <f aca="false">Defaults!A4</f>
-        <v>Emission duration</v>
-      </c>
-      <c r="B16" s="10" t="s">
-        <v>138</v>
-      </c>
-    </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="59" t="str">
-        <f aca="false">Defaults!A5</f>
-        <v>Application rate</v>
-      </c>
-      <c r="B17" s="18" t="s">
-        <v>130</v>
-      </c>
+      <c r="A17" s="63"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="59"/>
+      <c r="A18" s="61" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="57" t="s">
-        <v>10</v>
+      <c r="A19" s="63" t="str">
+        <f aca="false">Settings!A2</f>
+        <v>Include input uncertainty?</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="59" t="str">
-        <f aca="false">Settings!A2</f>
+      <c r="A20" s="63" t="str">
+        <f aca="false">Settings!A3</f>
+        <v>Include par uncertainty?</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="63" t="str">
+        <f aca="false">Settings!A4</f>
+        <v>Uncertainty iterations</v>
+      </c>
+      <c r="B21" s="18" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="63" t="str">
+        <f aca="false">Settings!A5</f>
+        <v>Confidence level</v>
+      </c>
+      <c r="B22" s="18" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="63" t="str">
+        <f aca="false">Settings!A6</f>
+        <v>Weather resolution</v>
+      </c>
+      <c r="B23" s="18" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="63" t="str">
+        <f aca="false">Settings!A7</f>
+        <v>Output digits</v>
+      </c>
+      <c r="B24" s="18" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="63" t="str">
+        <f aca="false">Settings!A8</f>
+        <v>Output file name</v>
+      </c>
+      <c r="B25" s="18" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="63" t="str">
+        <f aca="false">Settings!A9</f>
+        <v>Overwrite output?</v>
+      </c>
+      <c r="B26" s="18" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="63" t="str">
+        <f aca="false">Settings!A10</f>
+        <v>Type of output</v>
+      </c>
+      <c r="B27" s="18" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="63"/>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="61" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="63" t="str">
+        <f aca="false">Reproducibility!A2</f>
         <v>Parameter set</v>
       </c>
-      <c r="B20" s="10" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="59" t="str">
-        <f aca="false">Settings!A3</f>
-        <v>Include input uncertainty?</v>
-      </c>
-      <c r="B21" s="10" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="59" t="str">
-        <f aca="false">Settings!A4</f>
-        <v>Include par uncertainty?</v>
-      </c>
-      <c r="B22" s="10" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="59" t="str">
-        <f aca="false">Settings!A5</f>
-        <v>Uncertainty iterations</v>
-      </c>
-      <c r="B23" s="18" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="59" t="str">
-        <f aca="false">Settings!A6</f>
+      <c r="B30" s="10" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="63" t="str">
+        <f aca="false">Reproducibility!A3</f>
         <v>Uncertainty seed</v>
       </c>
-      <c r="B24" s="18" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="59" t="str">
-        <f aca="false">Settings!A7</f>
-        <v>Confidence level</v>
-      </c>
-      <c r="B25" s="18" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="59" t="str">
-        <f aca="false">Settings!A8</f>
-        <v>Weather type</v>
-      </c>
-      <c r="B26" s="18" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="59" t="str">
-        <f aca="false">Settings!A9</f>
-        <v>Output digits</v>
-      </c>
-      <c r="B27" s="18" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="59" t="str">
-        <f aca="false">Settings!A10</f>
-        <v>Output file name</v>
-      </c>
-      <c r="B28" s="18" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="59" t="str">
-        <f aca="false">Settings!A11</f>
-        <v>Overwrite output?</v>
-      </c>
-      <c r="B29" s="18" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="59" t="str">
-        <f aca="false">Settings!A12</f>
-        <v>Type of output</v>
-      </c>
-      <c r="B30" s="18" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="59"/>
+      <c r="B31" s="18" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="57" t="s">
-        <v>111</v>
+      <c r="A32" s="63" t="str">
+        <f aca="false">Reproducibility!A4</f>
+        <v>Emission duration (h)</v>
+      </c>
+      <c r="B32" s="10" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="59"/>
+      <c r="A33" s="63"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="59"/>
+      <c r="A34" s="63"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="59"/>
+      <c r="A35" s="63"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="59"/>
+      <c r="A36" s="63"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="59"/>
+      <c r="A37" s="63"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="59"/>
+      <c r="A38" s="63"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="59"/>
+      <c r="A39" s="63"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="59"/>
+      <c r="A40" s="63"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="59"/>
-    </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="59"/>
-    </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="59"/>
-    </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="59"/>
+      <c r="A41" s="63"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1798,7 +1903,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -1806,10 +1911,10 @@
   <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K16" activeCellId="0" sqref="K16"/>
+      <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.33"/>
@@ -1818,35 +1923,35 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="13.65"/>
   </cols>
   <sheetData>
-    <row r="1" s="61" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="61" t="s">
-        <v>150</v>
-      </c>
-      <c r="C1" s="61" t="s">
-        <v>151</v>
-      </c>
-      <c r="E1" s="61" t="s">
-        <v>152</v>
-      </c>
-      <c r="G1" s="61" t="s">
-        <v>153</v>
-      </c>
-      <c r="I1" s="61" t="s">
-        <v>154</v>
-      </c>
-      <c r="K1" s="61" t="s">
-        <v>155</v>
+    <row r="1" s="65" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="65" t="s">
+        <v>157</v>
+      </c>
+      <c r="C1" s="65" t="s">
+        <v>158</v>
+      </c>
+      <c r="E1" s="65" t="s">
+        <v>159</v>
+      </c>
+      <c r="G1" s="65" t="s">
+        <v>160</v>
+      </c>
+      <c r="I1" s="65" t="s">
+        <v>161</v>
+      </c>
+      <c r="K1" s="65" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>156</v>
+        <v>163</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>157</v>
+        <v>164</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>158</v>
+        <v>165</v>
       </c>
       <c r="G2" s="0" t="s">
         <v>65</v>
@@ -1855,35 +1960,38 @@
         <v>69</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>159</v>
+        <v>166</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>160</v>
+        <v>167</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>161</v>
+        <v>168</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>57</v>
+        <v>111</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>72</v>
+        <v>169</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>162</v>
+        <v>170</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>164</v>
+        <v>172</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>173</v>
       </c>
       <c r="K4" s="0" t="s">
         <v>71</v>
@@ -1891,18 +1999,18 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>165</v>
+        <v>174</v>
       </c>
       <c r="K5" s="0" t="s">
-        <v>166</v>
+        <v>175</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>167</v>
+        <v>176</v>
       </c>
       <c r="K6" s="0" t="s">
-        <v>168</v>
+        <v>177</v>
       </c>
     </row>
   </sheetData>
@@ -1939,13 +2047,13 @@
   <sheetData>
     <row r="1" s="14" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="13" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D1" s="14" t="s">
         <v>3</v>
@@ -1997,19 +2105,19 @@
   <sheetData>
     <row r="1" s="14" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="13" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" s="14" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2052,11 +2160,11 @@
   <dimension ref="A1:AMJ35"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="I3" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topRight" activeCell="I1" activeCellId="0" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2081,62 +2189,62 @@
   <sheetData>
     <row r="1" s="14" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="14" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="F1" s="14" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="G1" s="14" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="H1" s="14" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="I1" s="24" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="J1" s="24" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="K1" s="14" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="L1" s="14" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="M1" s="14" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="N1" s="14" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="AMI1" s="1"/>
       <c r="AMJ1" s="1"/>
     </row>
     <row r="2" s="14" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="14" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="E2" s="25" t="str">
         <f aca="false">Units!B2</f>
@@ -2155,23 +2263,23 @@
         <v>t/ha</v>
       </c>
       <c r="I2" s="24" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="J2" s="24" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="K2" s="14" t="str">
         <f aca="false">Units!B8</f>
         <v>kg/t</v>
       </c>
       <c r="L2" s="14" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="M2" s="14" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="N2" s="14" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="AMI2" s="1"/>
       <c r="AMJ2" s="1"/>
@@ -2501,10 +2609,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2516,108 +2624,90 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="31" t="s">
-        <v>56</v>
-      </c>
-      <c r="B2" s="32" t="s">
-        <v>57</v>
+      <c r="A2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" s="31" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B3" s="33" t="s">
-        <v>59</v>
+        <v>61</v>
+      </c>
+      <c r="B3" s="32" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B4" s="33" t="s">
-        <v>59</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="B4" s="33"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B5" s="34"/>
+        <v>63</v>
+      </c>
+      <c r="B5" s="33"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B6" s="34"/>
+        <v>64</v>
+      </c>
+      <c r="B6" s="32" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B7" s="34"/>
+        <v>66</v>
+      </c>
+      <c r="B7" s="33" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B8" s="33" t="s">
-        <v>65</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="B8" s="33"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B9" s="34" t="n">
-        <v>4</v>
+        <v>68</v>
+      </c>
+      <c r="B9" s="32" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B10" s="34"/>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B11" s="33" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B12" s="35" t="s">
+      <c r="B10" s="34" t="s">
         <v>71</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="4">
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B2" type="list">
-      <formula1>Options!$E$2:$E$4</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B3:B4 B11" type="list">
+  <dataValidations count="3">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B2:B3 B9" type="list">
       <formula1>Options!$I$2:$I$3</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B8" type="list">
-      <formula1>Options!$G$2:$G$3</formula1>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B10" type="list">
+      <formula1>Options!$K$2:$K$7</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B12" type="list">
-      <formula1>Options!$K$2:$K$7</formula1>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B6" type="list">
+      <formula1>Options!$G$2:$G$4</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -2665,46 +2755,46 @@
       <c r="A2" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B2" s="36" t="s">
+      <c r="B2" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="C2" s="37"/>
+      <c r="C2" s="36"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B3" s="38" t="s">
+      <c r="B3" s="37" t="s">
         <v>76</v>
       </c>
-      <c r="C3" s="39"/>
+      <c r="C3" s="38"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B4" s="38" t="s">
+      <c r="B4" s="37" t="s">
         <v>79</v>
       </c>
-      <c r="C4" s="39"/>
+      <c r="C4" s="38"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B5" s="38" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" s="37" t="s">
         <v>80</v>
       </c>
-      <c r="C5" s="39"/>
+      <c r="C5" s="38"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B6" s="38" t="s">
+      <c r="B6" s="37" t="s">
         <v>82</v>
       </c>
-      <c r="C6" s="39" t="s">
+      <c r="C6" s="38" t="s">
         <v>83</v>
       </c>
     </row>
@@ -2712,37 +2802,37 @@
       <c r="A7" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B7" s="38" t="s">
+      <c r="B7" s="37" t="s">
         <v>85</v>
       </c>
-      <c r="C7" s="39"/>
+      <c r="C7" s="38"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B8" s="38" t="s">
+      <c r="B8" s="37" t="s">
         <v>85</v>
       </c>
-      <c r="C8" s="39"/>
+      <c r="C8" s="38"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B9" s="40" t="s">
+      <c r="B9" s="39" t="s">
         <v>88</v>
       </c>
-      <c r="C9" s="39"/>
+      <c r="C9" s="38"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B10" s="41" t="s">
+      <c r="B10" s="40" t="s">
         <v>90</v>
       </c>
-      <c r="C10" s="42"/>
+      <c r="C10" s="41"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E20" s="1" t="s">
@@ -2775,7 +2865,8 @@
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="12" width="23.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="12" width="23.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="12" width="25.21"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="5" style="12" width="11.52"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="7" style="1" width="11.57"/>
   </cols>
@@ -2811,63 +2902,63 @@
         <f aca="false">Units!B6</f>
         <v>% FM</v>
       </c>
-      <c r="C2" s="43"/>
+      <c r="C2" s="42"/>
       <c r="D2" s="16"/>
       <c r="E2" s="16"/>
       <c r="F2" s="16"/>
-      <c r="G2" s="37"/>
+      <c r="G2" s="36"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="C3" s="44"/>
+      <c r="C3" s="43"/>
       <c r="D3" s="18"/>
       <c r="E3" s="18"/>
       <c r="F3" s="18"/>
-      <c r="G3" s="39"/>
+      <c r="G3" s="38"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B4" s="25" t="str">
         <f aca="false">Units!B5</f>
         <v>t/ha</v>
       </c>
-      <c r="C4" s="44"/>
+      <c r="C4" s="43"/>
       <c r="D4" s="18"/>
       <c r="E4" s="18"/>
       <c r="F4" s="18"/>
-      <c r="G4" s="39"/>
+      <c r="G4" s="38"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B5" s="25" t="str">
         <f aca="false">Units!B2</f>
         <v>t</v>
       </c>
-      <c r="C5" s="44"/>
+      <c r="C5" s="43"/>
       <c r="D5" s="18"/>
       <c r="E5" s="18"/>
       <c r="F5" s="18"/>
-      <c r="G5" s="39"/>
+      <c r="G5" s="38"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B6" s="25" t="str">
         <f aca="false">Units!B8</f>
         <v>kg/t</v>
       </c>
-      <c r="C6" s="44"/>
+      <c r="C6" s="43"/>
       <c r="D6" s="18"/>
       <c r="E6" s="18"/>
       <c r="F6" s="18"/>
-      <c r="G6" s="39"/>
+      <c r="G6" s="38"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
@@ -2877,11 +2968,11 @@
         <f aca="false">Units!B9</f>
         <v>°C</v>
       </c>
-      <c r="C7" s="44"/>
+      <c r="C7" s="43"/>
       <c r="D7" s="18"/>
       <c r="E7" s="18"/>
       <c r="F7" s="18"/>
-      <c r="G7" s="39"/>
+      <c r="G7" s="38"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
@@ -2891,11 +2982,11 @@
         <f aca="false">Units!B10</f>
         <v>m/s</v>
       </c>
-      <c r="C8" s="45"/>
-      <c r="D8" s="46"/>
-      <c r="E8" s="46"/>
-      <c r="F8" s="46"/>
-      <c r="G8" s="42"/>
+      <c r="C8" s="44"/>
+      <c r="D8" s="45"/>
+      <c r="E8" s="45"/>
+      <c r="F8" s="45"/>
+      <c r="G8" s="41"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2913,10 +3004,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2924,8 +3015,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="12" width="25.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="12" width="23.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="12" width="17.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="47" width="12.68"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="5" style="12" width="11.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="46" width="12.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="46" width="30.66"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="6" style="12" width="11.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2938,102 +3030,109 @@
       <c r="C1" s="14" t="s">
         <v>99</v>
       </c>
-      <c r="D1" s="48" t="s">
+      <c r="D1" s="47" t="s">
         <v>100</v>
       </c>
+      <c r="E1" s="47" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="49" t="s">
-        <v>101</v>
-      </c>
-      <c r="B2" s="49" t="s">
-        <v>53</v>
-      </c>
-      <c r="C2" s="50"/>
-      <c r="D2" s="47" t="n">
+      <c r="A2" s="48" t="s">
+        <v>102</v>
+      </c>
+      <c r="B2" s="48" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" s="49"/>
+      <c r="D2" s="46" t="n">
         <v>15</v>
       </c>
+      <c r="E2" s="46" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="51" t="s">
-        <v>102</v>
-      </c>
-      <c r="B3" s="51" t="s">
-        <v>103</v>
-      </c>
-      <c r="C3" s="52"/>
-      <c r="D3" s="53" t="s">
+      <c r="A3" s="50" t="s">
         <v>104</v>
       </c>
+      <c r="B3" s="50" t="s">
+        <v>105</v>
+      </c>
+      <c r="C3" s="51"/>
+      <c r="D3" s="52" t="s">
+        <v>106</v>
+      </c>
+      <c r="E3" s="46" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="51" t="s">
-        <v>105</v>
+      <c r="A4" s="12" t="s">
+        <v>46</v>
       </c>
       <c r="B4" s="25" t="str">
-        <f aca="false">Units!B8</f>
-        <v>kg/t</v>
-      </c>
-      <c r="C4" s="34"/>
-      <c r="D4" s="47" t="n">
-        <v>168</v>
-      </c>
+        <f aca="false">Units!B5</f>
+        <v>t/ha</v>
+      </c>
+      <c r="C4" s="33"/>
+      <c r="D4" s="46" t="n">
+        <v>40</v>
+      </c>
+      <c r="E4" s="53" t="s">
+        <v>108</v>
+      </c>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="12" t="s">
-        <v>43</v>
+        <v>81</v>
       </c>
       <c r="B5" s="25" t="str">
-        <f aca="false">Units!B5</f>
-        <v>t/ha</v>
-      </c>
-      <c r="C5" s="34"/>
-      <c r="D5" s="47" t="n">
-        <v>40</v>
-      </c>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
+        <f aca="false">Units!B6</f>
+        <v>% FM</v>
+      </c>
+      <c r="C5" s="54"/>
+      <c r="D5" s="46" t="n">
+        <v>5</v>
+      </c>
+      <c r="E5" s="53" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="B6" s="25" t="str">
-        <f aca="false">Units!B6</f>
-        <v>% FM</v>
-      </c>
-      <c r="C6" s="54"/>
-      <c r="D6" s="47" t="n">
-        <v>5</v>
+        <v>98</v>
+      </c>
+      <c r="B6" s="25"/>
+      <c r="C6" s="33"/>
+      <c r="D6" s="46" t="n">
+        <v>7</v>
+      </c>
+      <c r="E6" s="53" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="12" t="s">
-        <v>98</v>
-      </c>
-      <c r="B7" s="25"/>
-      <c r="C7" s="34"/>
-      <c r="D7" s="47" t="n">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="12" t="s">
-        <v>106</v>
-      </c>
-      <c r="B8" s="25" t="str">
+        <v>109</v>
+      </c>
+      <c r="B7" s="25" t="str">
         <f aca="false">Units!B7</f>
         <v>kg/t</v>
       </c>
-      <c r="C8" s="55"/>
-      <c r="D8" s="47" t="n">
+      <c r="C7" s="55"/>
+      <c r="D7" s="46" t="n">
         <v>3</v>
+      </c>
+      <c r="E7" s="53" t="s">
+        <v>108</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C6" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C5" type="list">
       <formula1>Options!$G$2:$G$3</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -3056,48 +3155,55 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.65234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.08"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="2" style="1" width="11.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="22.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="12" width="15.58"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="3" style="1" width="11.77"/>
   </cols>
   <sheetData>
-    <row r="1" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>108</v>
+        <v>57</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="36" t="s">
-        <v>109</v>
-      </c>
-      <c r="B2" s="37" t="s">
+      <c r="A2" s="56" t="s">
         <v>110</v>
       </c>
+      <c r="B2" s="57" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="38" t="s">
-        <v>111</v>
-      </c>
-      <c r="B3" s="39" t="s">
+      <c r="A3" s="1" t="s">
         <v>112</v>
       </c>
+      <c r="B3" s="58" t="n">
+        <v>120178</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="41" t="s">
+      <c r="A4" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B4" s="42" t="s">
-        <v>114</v>
+      <c r="B4" s="59" t="n">
+        <v>168</v>
       </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B2" type="list">
+      <formula1>Options!$E$2:$E$4</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>